<commit_message>
spin that shit :weary:
</commit_message>
<xml_diff>
--- a/WebServices (Without SP)/1400/08_آبان/راهنمای وب سرویس_ ثبت درخواست اولیه خاموشی بابرنامه14000319.xlsx
+++ b/WebServices (Without SP)/1400/08_آبان/راهنمای وب سرویس_ ثبت درخواست اولیه خاموشی بابرنامه14000319.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dadvar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\WebServices (Without SP)\1400\08_آبان\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFEEDA9-2A9A-4006-ADC7-44C33ED58E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B01327-9877-41D0-9775-ED46FBAEF3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="وب سرویس ثبت حادثه" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'وب سرویس ثبت حادثه'!$A$1:$D$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'وب سرویس ثبت حادثه'!$A$1:$D$38</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="83">
   <si>
     <t>int</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>وضعیت کار در مناطق شهری</t>
-  </si>
-  <si>
-    <t>نوع شبکه (MP: فشار متوسط، LP : فشار ضعیف)</t>
   </si>
   <si>
     <t>تاریخ درخواست قطع</t>
@@ -332,6 +329,15 @@
   </si>
   <si>
     <t xml:space="preserve"> کار در خط گرم</t>
+  </si>
+  <si>
+    <t>NetworkTypeId</t>
+  </si>
+  <si>
+    <t>نوع شبکه (2: فشار متوسط، 3 : فشار ضعیف) -- درصورتی که NetworkType نباشد، اجباری است.</t>
+  </si>
+  <si>
+    <t>نوع شبکه (MP: فشار متوسط، LP : فشار ضعیف) -- -- درصورتی که NetworkTypeId داشته باشیم، اختیاری است.</t>
   </si>
 </sst>
 </file>
@@ -757,7 +763,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -844,6 +850,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,8 +937,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1335,10 +1344,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,32 +1358,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="40"/>
+      <c r="A1" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="45"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
@@ -1383,10 +1392,10 @@
       <c r="B4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="47"/>
+      <c r="C4" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="48"/>
     </row>
     <row r="5" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1403,12 +1412,12 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
     </row>
     <row r="7" spans="1:4" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -1516,7 +1525,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>5</v>
@@ -1530,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>5</v>
@@ -1544,7 +1553,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>5</v>
@@ -1558,7 +1567,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>5</v>
@@ -1588,7 +1597,7 @@
       <c r="C19" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="58" t="s">
+      <c r="D19" s="30" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1600,7 +1609,7 @@
         <v>49</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>5</v>
@@ -1658,7 +1667,7 @@
       <c r="C24" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="58" t="s">
+      <c r="D24" s="30" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1672,7 +1681,7 @@
       <c r="C25" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="58" t="s">
+      <c r="D25" s="30" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1692,139 +1701,153 @@
     </row>
     <row r="27" spans="1:4" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B28" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="C28" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B29" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="C29" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="51" t="s">
+    <row r="31" spans="1:4" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="53"/>
-    </row>
-    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="55"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="54"/>
     </row>
     <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="56"/>
+    </row>
+    <row r="34" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C34" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="55"/>
-    </row>
-    <row r="34" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
+      <c r="D34" s="56"/>
+    </row>
+    <row r="35" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C35" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="57"/>
-    </row>
-    <row r="35" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="30" t="s">
+      <c r="D35" s="58"/>
+    </row>
+    <row r="36" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="32" t="s">
+      <c r="B36" s="32"/>
+      <c r="C36" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="33"/>
-    </row>
-    <row r="36" spans="1:4" ht="399.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="37"/>
+      <c r="D36" s="34"/>
+    </row>
+    <row r="37" spans="1:4" ht="399.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="36"/>
+      <c r="C37" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>